<commit_message>
Added match defense saving
</commit_message>
<xml_diff>
--- a/docs/Reference.xlsx
+++ b/docs/Reference.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="13395" windowHeight="11070"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="13395" windowHeight="11070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
+    <sheet name="Defenses" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="145">
   <si>
     <t>Button Label</t>
   </si>
@@ -407,6 +408,48 @@
   </si>
   <si>
     <t>$fouls</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Portcullis</t>
+  </si>
+  <si>
+    <t>Cheval</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Moat</t>
+  </si>
+  <si>
+    <t>Ramparts</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Drawbridge</t>
+  </si>
+  <si>
+    <t>Sally Port</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Rock Wall</t>
+  </si>
+  <si>
+    <t>Rough Terrain</t>
   </si>
 </sst>
 </file>
@@ -785,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -1325,4 +1368,132 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2">
+        <f>LEN(B2)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C10" si="0">LEN(B3)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing deploy to new server
</commit_message>
<xml_diff>
--- a/docs/Reference.xlsx
+++ b/docs/Reference.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="13395" windowHeight="11070" activeTab="1"/>
+    <workbookView xWindow="3405" yWindow="90" windowWidth="13395" windowHeight="7455" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
     <sheet name="Defenses" sheetId="2" r:id="rId2"/>
+    <sheet name="matchScore" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="257">
   <si>
     <t>Button Label</t>
   </si>
@@ -450,13 +451,349 @@
   </si>
   <si>
     <t>Rough Terrain</t>
+  </si>
+  <si>
+    <t>&lt;/z:anyType&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   &lt;/MatchScores&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/Score_2016&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;/Alliances&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;/Alliance&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;towerFaceC /&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;towerFaceB /&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;towerFaceA /&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;towerEndStrength&gt;0&lt;/towerEndStrength&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;totalPoints&gt;0&lt;/totalPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;teleopTowerCaptured&gt;false&lt;/teleopTowerCaptured&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;teleopScalePoints&gt;0&lt;/teleopScalePoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;teleopPoints&gt;0&lt;/teleopPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;teleopDefensesBreached&gt;true&lt;/teleopDefensesBreached&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;teleopCrossingPoints&gt;0&lt;/teleopCrossingPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;teleopChallengePoints&gt;0&lt;/teleopChallengePoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;teleopBouldersLow&gt;0&lt;/teleopBouldersLow&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;teleopBouldersHigh&gt;0&lt;/teleopBouldersHigh&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;teleopBoulderPoints&gt;0&lt;/teleopBoulderPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;techFoulCount&gt;0&lt;/techFoulCount&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;robot3Auto&gt;Challenged&lt;/robot3Auto&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;robot2Auto&gt;Both&lt;/robot2Auto&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;robot1Auto&gt;None&lt;/robot1Auto&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position5crossings&gt;0&lt;/position5crossings&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position5&gt;D_RoughTerrain&lt;/position5&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position4crossings&gt;2&lt;/position4crossings&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position4&gt;C_Drawbridge&lt;/position4&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position3crossings&gt;2&lt;/position3crossings&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position3&gt;B_Moat&lt;/position3&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position2crossings&gt;2&lt;/position2crossings&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position2&gt;A_ChevalDeFrise&lt;/position2&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position1crossings&gt;2&lt;/position1crossings&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;foulPoints&gt;0&lt;/foulPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;foulCount&gt;0&lt;/foulCount&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;capturePoints&gt;0&lt;/capturePoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;breachPoints&gt;0&lt;/breachPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;autoReachPoints&gt;0&lt;/autoReachPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;autoPoints&gt;0&lt;/autoPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;autoCrossingPoints&gt;0&lt;/autoCrossingPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;autoBouldersLow&gt;0&lt;/autoBouldersLow&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;autoBouldersHigh&gt;0&lt;/autoBouldersHigh&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;autoBoulderPoints&gt;0&lt;/autoBoulderPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;alliance&gt;Red&lt;/alliance&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;adjustPoints&gt;0&lt;/adjustPoints&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;Alliance&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;towerFaceC&gt;Scaled&lt;/towerFaceC&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;towerFaceB&gt;Scaled&lt;/towerFaceB&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;towerFaceA&gt;None&lt;/towerFaceA&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;teleopDefensesBreached&gt;false&lt;/teleopDefensesBreached&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;robot3Auto&gt;Reached&lt;/robot3Auto&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;robot2Auto&gt;Reached&lt;/robot2Auto&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position5crossings&gt;1&lt;/position5crossings&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position5&gt;D_RockWall&lt;/position5&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position4crossings&gt;1&lt;/position4crossings&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position4&gt;C_SallyPort&lt;/position4&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position3crossings&gt;0&lt;/position3crossings&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position3&gt;B_Ramparts&lt;/position3&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position2crossings&gt;1&lt;/position2crossings&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;position2&gt;A_Portcullis&lt;/position2&gt;</t>
+  </si>
+  <si>
+    <t>autoBoulderPoints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               &lt;alliance&gt;Blue&lt;/alliance&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;Alliances&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;matchNumber&gt;1&lt;/matchNumber&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;matchLevel&gt;Qualification&lt;/matchLevel&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;AudienceGroup&gt;GroupA&lt;/AudienceGroup&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;Score_2016&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   &lt;MatchScores&gt;</t>
+  </si>
+  <si>
+    <t>&lt;z:anyType xmlns:z="http://schemas.microsoft.com/2003/10/Serialization/" xmlns:i="http://www.w3.org/2001/XMLSchema-instance" i:type="EventScoreDetails"&gt;</t>
+  </si>
+  <si>
+    <t>autoBouldersLow</t>
+  </si>
+  <si>
+    <t>autoBouldersHigh</t>
+  </si>
+  <si>
+    <t>autoCrossingPoints</t>
+  </si>
+  <si>
+    <t>autoPoints</t>
+  </si>
+  <si>
+    <t>autoReachPoints</t>
+  </si>
+  <si>
+    <t>breachPoints</t>
+  </si>
+  <si>
+    <t>capturePoints</t>
+  </si>
+  <si>
+    <t>foulCount</t>
+  </si>
+  <si>
+    <t>foulPoints</t>
+  </si>
+  <si>
+    <t>position1crossings</t>
+  </si>
+  <si>
+    <t>position2</t>
+  </si>
+  <si>
+    <t>position2crossings</t>
+  </si>
+  <si>
+    <t>A_Portcullis</t>
+  </si>
+  <si>
+    <t>B_Ramparts</t>
+  </si>
+  <si>
+    <t>position3</t>
+  </si>
+  <si>
+    <t>C_SallyPort</t>
+  </si>
+  <si>
+    <t>D_RockWall</t>
+  </si>
+  <si>
+    <t>position3crossings</t>
+  </si>
+  <si>
+    <t>position4</t>
+  </si>
+  <si>
+    <t>position4crossings</t>
+  </si>
+  <si>
+    <t>position5</t>
+  </si>
+  <si>
+    <t>position5crossings</t>
+  </si>
+  <si>
+    <t>robot1Auto</t>
+  </si>
+  <si>
+    <t>robot2Auto</t>
+  </si>
+  <si>
+    <t>robot3Auto</t>
+  </si>
+  <si>
+    <t>techFoulCount</t>
+  </si>
+  <si>
+    <t>teleopBoulderPoints</t>
+  </si>
+  <si>
+    <t>teleopBouldersHigh</t>
+  </si>
+  <si>
+    <t>teleopBouldersLow</t>
+  </si>
+  <si>
+    <t>teleopChallengePoints</t>
+  </si>
+  <si>
+    <t>teleopCrossingPoints</t>
+  </si>
+  <si>
+    <t>teleopDefensesBreached</t>
+  </si>
+  <si>
+    <t>teleopPoints</t>
+  </si>
+  <si>
+    <t>teleopScalePoints</t>
+  </si>
+  <si>
+    <t>teleopTowerCaptured</t>
+  </si>
+  <si>
+    <t>totalPoints</t>
+  </si>
+  <si>
+    <t>towerEndStrength</t>
+  </si>
+  <si>
+    <t>towerFaceA</t>
+  </si>
+  <si>
+    <t>towerFaceB</t>
+  </si>
+  <si>
+    <t>towerFaceC</t>
+  </si>
+  <si>
+    <t>A_ChevalDeFrise</t>
+  </si>
+  <si>
+    <t>B_Moat</t>
+  </si>
+  <si>
+    <t>C_Drawbridge</t>
+  </si>
+  <si>
+    <t>D_RoughTerrain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +808,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Source Code Pro"/>
     </font>
   </fonts>
   <fills count="4">
@@ -520,11 +867,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,7 +965,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -649,7 +999,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -825,14 +1174,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -843,7 +1192,7 @@
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -866,7 +1215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -889,7 +1238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -910,7 +1259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
@@ -931,7 +1280,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -952,7 +1301,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
@@ -973,7 +1322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -996,7 +1345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
@@ -1019,7 +1368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -1042,7 +1391,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>56</v>
       </c>
@@ -1065,7 +1414,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>60</v>
       </c>
@@ -1088,7 +1437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -1111,7 +1460,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>68</v>
       </c>
@@ -1134,7 +1483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>72</v>
       </c>
@@ -1157,7 +1506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>76</v>
       </c>
@@ -1180,7 +1529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="3" t="s">
         <v>82</v>
       </c>
@@ -1203,7 +1552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>84</v>
       </c>
@@ -1226,7 +1575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>88</v>
       </c>
@@ -1249,7 +1598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
         <v>91</v>
       </c>
@@ -1272,7 +1621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
         <v>94</v>
       </c>
@@ -1295,7 +1644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
         <v>98</v>
       </c>
@@ -1318,7 +1667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="2" t="s">
         <v>102</v>
       </c>
@@ -1341,7 +1690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
         <v>105</v>
       </c>
@@ -1371,19 +1720,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -1391,7 +1740,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -1403,7 +1752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -1415,7 +1764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -1427,7 +1776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -1439,7 +1788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -1451,7 +1800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -1463,7 +1812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -1475,7 +1824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -1487,7 +1836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="C10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1496,4 +1845,627 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="23.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added robot death stat
</commit_message>
<xml_diff>
--- a/docs/Reference.xlsx
+++ b/docs/Reference.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="90" windowWidth="13395" windowHeight="7455" activeTab="2"/>
+    <workbookView xWindow="450" yWindow="705" windowWidth="13395" windowHeight="7455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
     <sheet name="Defenses" sheetId="2" r:id="rId2"/>
     <sheet name="matchScore" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="266">
   <si>
     <t>Button Label</t>
   </si>
@@ -787,12 +787,39 @@
   </si>
   <si>
     <t>D_RoughTerrain</t>
+  </si>
+  <si>
+    <t>died_btn</t>
+  </si>
+  <si>
+    <t>died</t>
+  </si>
+  <si>
+    <t>Died</t>
+  </si>
+  <si>
+    <t>died_badge</t>
+  </si>
+  <si>
+    <t>$died</t>
+  </si>
+  <si>
+    <t>Name Length</t>
+  </si>
+  <si>
+    <t>API Name</t>
+  </si>
+  <si>
+    <t>API Name Length</t>
+  </si>
+  <si>
+    <t>Max Length</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -840,7 +867,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -863,11 +890,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -876,6 +914,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,6 +1008,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -999,6 +1043,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1174,11 +1219,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1713,6 +1758,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1720,139 +1788,220 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <f>LEN(B2)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="D2" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="2">
+        <f>LEN(D2)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C10" si="0">LEN(B3)</f>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:E9" si="0">LEN(B3)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="D3" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="D4" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="D5" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="D6" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="D7" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="D8" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="C10">
+      <c r="D9" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="10">
+        <f>MAX(C2:C9)</f>
+        <v>13</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="10">
+        <f>MAX(E2:E9)</f>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Separated current match and defenses
</commit_message>
<xml_diff>
--- a/docs/Reference.xlsx
+++ b/docs/Reference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="705" windowWidth="13395" windowHeight="7455" activeTab="1"/>
+    <workbookView xWindow="450" yWindow="705" windowWidth="13395" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="274">
   <si>
     <t>Button Label</t>
   </si>
@@ -814,6 +814,30 @@
   </si>
   <si>
     <t>Max Length</t>
+  </si>
+  <si>
+    <t>red_def2</t>
+  </si>
+  <si>
+    <t>red_def3</t>
+  </si>
+  <si>
+    <t>red_def4</t>
+  </si>
+  <si>
+    <t>red_def5</t>
+  </si>
+  <si>
+    <t>blue_def2</t>
+  </si>
+  <si>
+    <t>blue_def3</t>
+  </si>
+  <si>
+    <t>blue_def4</t>
+  </si>
+  <si>
+    <t>blue_def5</t>
   </si>
 </sst>
 </file>
@@ -1220,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1781,6 +1805,70 @@
         <v>8</v>
       </c>
     </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>266</v>
+      </c>
+      <c r="B27" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>267</v>
+      </c>
+      <c r="B28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>268</v>
+      </c>
+      <c r="B29" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>269</v>
+      </c>
+      <c r="B30" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>270</v>
+      </c>
+      <c r="B31" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>271</v>
+      </c>
+      <c r="B32" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>272</v>
+      </c>
+      <c r="B33" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>273</v>
+      </c>
+      <c r="B34" t="s">
+        <v>273</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1791,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Match results are loading now
</commit_message>
<xml_diff>
--- a/docs/Reference.xlsx
+++ b/docs/Reference.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="705" windowWidth="13395" windowHeight="7455" activeTab="2"/>
+    <workbookView xWindow="450" yWindow="705" windowWidth="13395" windowHeight="7455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
     <sheet name="Defenses" sheetId="2" r:id="rId2"/>
     <sheet name="matchScore" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="334">
   <si>
     <t>Button Label</t>
   </si>
@@ -991,12 +991,39 @@
   </si>
   <si>
     <t>blue_tower_3_status</t>
+  </si>
+  <si>
+    <t>avg_cross_low_bar</t>
+  </si>
+  <si>
+    <t>avg_cross_portcullis</t>
+  </si>
+  <si>
+    <t>avg_cross_cheval</t>
+  </si>
+  <si>
+    <t>avg_cross_ramparts</t>
+  </si>
+  <si>
+    <t>avg_cross_moat</t>
+  </si>
+  <si>
+    <t>avg_cross_sallyport</t>
+  </si>
+  <si>
+    <t>avg_cross_drawbridge</t>
+  </si>
+  <si>
+    <t>avg_cross_rockwall</t>
+  </si>
+  <si>
+    <t>avg_cross_rough</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -1100,8 +1127,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1185,7 +1240,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1220,7 +1274,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1396,7 +1449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2029,11 +2082,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2046,7 +2099,7 @@
     <col min="6" max="6" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2062,8 +2115,11 @@
       <c r="E1" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>133</v>
       </c>
@@ -2081,8 +2137,11 @@
         <f>LEN(D2)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>133</v>
       </c>
@@ -2100,8 +2159,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>136</v>
       </c>
@@ -2119,8 +2181,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>136</v>
       </c>
@@ -2138,8 +2203,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>139</v>
       </c>
@@ -2157,8 +2225,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>139</v>
       </c>
@@ -2176,8 +2247,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>142</v>
       </c>
@@ -2195,8 +2269,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>142</v>
       </c>
@@ -2214,8 +2291,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>265</v>
       </c>
@@ -2238,10 +2318,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
+    <sheetView topLeftCell="E17" workbookViewId="0">
       <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>

</xml_diff>